<commit_message>
Frontend Arbeitspakete für Resourcenplan
</commit_message>
<xml_diff>
--- a/Documents/Ressourcenplan.xlsx
+++ b/Documents/Ressourcenplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WebEngineering2\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\PycharmProjects\WebEngineering2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECBA6D3-3007-470F-A664-416A10A55824}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9199A868-07EF-4202-AB41-34441DA8E967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D8609A72-7219-446E-A826-8B026BDFADC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D8609A72-7219-446E-A826-8B026BDFADC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -45,9 +56,6 @@
     <t>Gesamtzeitdauer:</t>
   </si>
   <si>
-    <t>Zeitdauer Viktoria</t>
-  </si>
-  <si>
     <t>Zeitdauer Noura</t>
   </si>
   <si>
@@ -66,9 +74,6 @@
     <t>Aufteilung der Arbeitspakete</t>
   </si>
   <si>
-    <t>Selina, Robin, Noura, Viktoria</t>
-  </si>
-  <si>
     <t>Entwicklung Backend</t>
   </si>
   <si>
@@ -163,6 +168,54 @@
   </si>
   <si>
     <t>Deployment, Testen der Anwendung</t>
+  </si>
+  <si>
+    <t>Selina, Robin, Noura, Victoria</t>
+  </si>
+  <si>
+    <t>Zeitdauer Victoria</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Noura, Victoria</t>
+  </si>
+  <si>
+    <t>Log In/Log Out</t>
+  </si>
+  <si>
+    <t>Noura</t>
+  </si>
+  <si>
+    <t>Merkliste</t>
+  </si>
+  <si>
+    <t>Nutzerprofil</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Angebot hinzufügen</t>
+  </si>
+  <si>
+    <t>Bilder hinzufügen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation durch die Website </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suche nach Artikeln </t>
+  </si>
+  <si>
+    <t>Navbar mit Kategorien und Unterkategorien</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Angebotanzeige nach Kategorie</t>
   </si>
 </sst>
 </file>
@@ -269,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -278,7 +331,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -287,7 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -296,6 +347,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -495,8 +552,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33A3B048-DE39-42D1-9A68-50A2A573DACB}" name="Tabelle1" displayName="Tabelle1" ref="A1:G33" totalsRowCount="1">
-  <autoFilter ref="A1:G32" xr:uid="{33A3B048-DE39-42D1-9A68-50A2A573DACB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33A3B048-DE39-42D1-9A68-50A2A573DACB}" name="Tabelle1" displayName="Tabelle1" ref="A1:G37" totalsRowShown="0">
+  <autoFilter ref="A1:G37" xr:uid="{33A3B048-DE39-42D1-9A68-50A2A573DACB}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B395AD55-E9D9-4AD5-B84E-9C09A77C9EE9}" name="Arbeitspaket" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{B1031F76-8EE3-49E7-BF63-90AF43F2F677}" name="Teilarbeitspakete" dataDxfId="5"/>
@@ -504,7 +561,7 @@
     <tableColumn id="6" xr3:uid="{A0D9738F-A332-4E79-97AA-16C9A1C10A32}" name="Zeitdauer Selina" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{55D08300-229F-47EB-A464-169FED7FC166}" name="Zeitdauer Robin" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{7C130676-3DB8-4EF6-8EB9-AED002553D65}" name="Zeitdauer Noura" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{972A3E60-72D4-40D0-BE76-B4739F411336}" name="Zeitdauer Viktoria" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{972A3E60-72D4-40D0-BE76-B4739F411336}" name="Zeitdauer Victoria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -807,28 +864,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E275EA-9F8C-4A51-A8DF-B5C7888A2144}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.81640625" customWidth="1"/>
-    <col min="2" max="2" width="37.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="65.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -837,22 +894,22 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3">
         <v>0.5</v>
@@ -867,13 +924,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3">
         <v>0.5</v>
@@ -892,13 +949,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -914,16 +971,16 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -937,410 +994,526 @@
       <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="10"/>
       <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="I6" s="15"/>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="I6" s="17"/>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="D7" s="7">
-        <v>3</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
       <c r="I7" s="5"/>
       <c r="J7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6">
+        <v>11.5</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6">
+        <v>3</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <v>5</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="6">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="14">
         <v>3</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="14">
+        <v>1</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="13">
+        <v>4</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16">
+        <f>SUM(D2:D36)</f>
+        <v>50</v>
+      </c>
+      <c r="E37" s="16">
+        <f>SUM(E2:E36)</f>
+        <v>40</v>
+      </c>
+      <c r="F37" s="19">
+        <f>SUM(F2:F36)</f>
         <v>3</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="7">
-        <v>10</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
-        <v>2</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7">
-        <v>10</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7">
-        <v>2</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7">
-        <v>2</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7">
-        <v>10</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7">
-        <v>3</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7">
-        <v>3</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7">
-        <v>5</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="7">
-        <v>5</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="7">
-        <v>3</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="16">
-        <v>3</v>
-      </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="16">
-        <v>1</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="15">
-        <v>4</v>
-      </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34">
-        <f>SUM(Tabelle1[Zeitdauer Selina])</f>
+      <c r="G37" s="16">
+        <f>SUM(G2:G36)</f>
         <v>50</v>
       </c>
-      <c r="E34">
-        <f>SUM(Tabelle1[Zeitdauer Robin])</f>
-        <v>40</v>
-      </c>
-      <c r="F34" s="6">
-        <f>SUM(Tabelle1[Zeitdauer Noura])</f>
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <f>SUM(Tabelle1[Zeitdauer Viktoria])</f>
-        <v>3</v>
-      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Made final changes for the deployment version of the app
</commit_message>
<xml_diff>
--- a/Documents/Ressourcenplan.xlsx
+++ b/Documents/Ressourcenplan.xlsx
@@ -5,31 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Personal Files\SynologyDrive\Studium\Projekte\WebEngineering2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4EFEB8-B5B2-4B15-9882-EB29CEB696D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B781C0-3FF9-48F4-AA6B-5FEEED679695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D8609A72-7219-446E-A826-8B026BDFADC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D8609A72-7219-446E-A826-8B026BDFADC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -866,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E275EA-9F8C-4A51-A8DF-B5C7888A2144}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,7 +1451,9 @@
         <v>24</v>
       </c>
       <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
+      <c r="E34" s="14">
+        <v>5</v>
+      </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
     </row>
@@ -1477,7 +1468,9 @@
       <c r="D35" s="14">
         <v>0.5</v>
       </c>
-      <c r="E35" s="14"/>
+      <c r="E35" s="14">
+        <v>0.5</v>
+      </c>
       <c r="F35" s="14">
         <v>0.5</v>
       </c>
@@ -1496,7 +1489,9 @@
       <c r="D36" s="13">
         <v>4</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="13">
+        <v>4.5</v>
+      </c>
       <c r="F36" s="13">
         <v>2.5</v>
       </c>
@@ -1516,7 +1511,7 @@
       </c>
       <c r="E37" s="16">
         <f>SUM(E2:E36)</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F37" s="19">
         <f>SUM(F2:F36)</f>

</xml_diff>